<commit_message>
Projeto atualizado, bug corrigido.
</commit_message>
<xml_diff>
--- a/static/dados_quiz.xlsx
+++ b/static/dados_quiz.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X3"/>
+  <dimension ref="A1:X9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -666,10 +666,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>71</t>
-        </is>
+      <c r="A3" t="n">
+        <v>71</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -746,44 +744,698 @@
           <t>nao</t>
         </is>
       </c>
-      <c r="Q3" t="inlineStr">
+      <c r="Q3" t="n">
+        <v>1</v>
+      </c>
+      <c r="R3" t="n">
+        <v>2</v>
+      </c>
+      <c r="S3" t="n">
+        <v>2</v>
+      </c>
+      <c r="T3" t="n">
+        <v>2</v>
+      </c>
+      <c r="U3" t="n">
+        <v>2</v>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>ruim</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>aprovado</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>aprovado</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>36</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="Q4" t="n">
+        <v>2</v>
+      </c>
+      <c r="R4" t="n">
+        <v>3</v>
+      </c>
+      <c r="S4" t="n">
+        <v>1</v>
+      </c>
+      <c r="T4" t="n">
+        <v>3</v>
+      </c>
+      <c r="U4" t="n">
+        <v>2</v>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>bom</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>reprovado</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>33</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="Q5" t="n">
+        <v>3</v>
+      </c>
+      <c r="R5" t="n">
+        <v>2</v>
+      </c>
+      <c r="S5" t="n">
+        <v>3</v>
+      </c>
+      <c r="T5" t="n">
+        <v>3</v>
+      </c>
+      <c r="U5" t="n">
+        <v>3</v>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>bom</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>reprovado</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>33</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="Q6" t="n">
+        <v>1</v>
+      </c>
+      <c r="R6" t="n">
+        <v>2</v>
+      </c>
+      <c r="S6" t="n">
+        <v>3</v>
+      </c>
+      <c r="T6" t="n">
+        <v>3</v>
+      </c>
+      <c r="U6" t="n">
+        <v>2</v>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>bom</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>reprovado</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>reprovado</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>33</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="Q7" t="n">
+        <v>1</v>
+      </c>
+      <c r="R7" t="n">
+        <v>1</v>
+      </c>
+      <c r="S7" t="n">
+        <v>1</v>
+      </c>
+      <c r="T7" t="n">
+        <v>3</v>
+      </c>
+      <c r="U7" t="n">
+        <v>3</v>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>bom</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>reprovado</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>reprovado</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>33</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="Q8" t="n">
+        <v>2</v>
+      </c>
+      <c r="R8" t="n">
+        <v>1</v>
+      </c>
+      <c r="S8" t="n">
+        <v>2</v>
+      </c>
+      <c r="T8" t="n">
+        <v>3</v>
+      </c>
+      <c r="U8" t="n">
+        <v>3</v>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>bom</t>
+        </is>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>reprovado</t>
+        </is>
+      </c>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>reprovado</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Prefiro não dizer</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="R3" t="inlineStr">
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="V3" t="inlineStr">
+      <c r="V9" t="inlineStr">
         <is>
           <t>ruim</t>
         </is>
       </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>aprovado</t>
-        </is>
-      </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>aprovado</t>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>reprovado</t>
+        </is>
+      </c>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>reprovado</t>
         </is>
       </c>
     </row>

</xml_diff>